<commit_message>
working days december run
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
+++ b/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495A8E6A-5C48-4F62-9BCA-49969A537ABF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC787C-1556-4DAD-8BE7-C43BEBE8D05C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="682">
   <si>
     <t>Test Case</t>
   </si>
@@ -2816,6 +2816,9 @@
   </si>
   <si>
     <t>january</t>
+  </si>
+  <si>
+    <t>december</t>
   </si>
 </sst>
 </file>
@@ -3192,7 +3195,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="91" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92:C541"/>
+      <selection pane="bottomLeft" activeCell="G200" sqref="G200:G541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10311,7 +10314,7 @@
         <v>210</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>211</v>
@@ -10391,7 +10394,7 @@
         <v>212</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>213</v>
@@ -10471,7 +10474,7 @@
         <v>214</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>215</v>
@@ -10791,7 +10794,7 @@
         <v>222</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>223</v>
@@ -10871,7 +10874,7 @@
         <v>224</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>225</v>
@@ -10951,7 +10954,7 @@
         <v>226</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>227</v>
@@ -11271,7 +11274,7 @@
         <v>234</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>235</v>
@@ -11351,7 +11354,7 @@
         <v>236</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>237</v>
@@ -11431,7 +11434,7 @@
         <v>238</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>239</v>
@@ -11511,7 +11514,7 @@
         <v>240</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>241</v>
@@ -11591,7 +11594,7 @@
         <v>242</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>243</v>
@@ -11671,7 +11674,7 @@
         <v>244</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>245</v>
@@ -18783,7 +18786,7 @@
         <v>678</v>
       </c>
       <c r="G200" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H200" s="4" t="s">
         <v>25</v>
@@ -18851,7 +18854,7 @@
         <v>212</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D201" s="4" t="s">
         <v>337</v>
@@ -18863,7 +18866,7 @@
         <v>678</v>
       </c>
       <c r="G201" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H201" s="4" t="s">
         <v>25</v>
@@ -18931,7 +18934,7 @@
         <v>214</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D202" s="4" t="s">
         <v>338</v>
@@ -18943,7 +18946,7 @@
         <v>678</v>
       </c>
       <c r="G202" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H202" s="4" t="s">
         <v>25</v>
@@ -19251,7 +19254,7 @@
         <v>222</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D206" s="4" t="s">
         <v>342</v>
@@ -19263,7 +19266,7 @@
         <v>678</v>
       </c>
       <c r="G206" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H206" s="4" t="s">
         <v>25</v>
@@ -19331,7 +19334,7 @@
         <v>224</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D207" s="4" t="s">
         <v>343</v>
@@ -19343,7 +19346,7 @@
         <v>678</v>
       </c>
       <c r="G207" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H207" s="4" t="s">
         <v>25</v>
@@ -19411,7 +19414,7 @@
         <v>226</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D208" s="4" t="s">
         <v>344</v>
@@ -19423,7 +19426,7 @@
         <v>678</v>
       </c>
       <c r="G208" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H208" s="4" t="s">
         <v>25</v>
@@ -19731,7 +19734,7 @@
         <v>234</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D212" s="4" t="s">
         <v>348</v>
@@ -19743,7 +19746,7 @@
         <v>678</v>
       </c>
       <c r="G212" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H212" s="4" t="s">
         <v>25</v>
@@ -19811,7 +19814,7 @@
         <v>236</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D213" s="4" t="s">
         <v>349</v>
@@ -19823,7 +19826,7 @@
         <v>678</v>
       </c>
       <c r="G213" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H213" s="4" t="s">
         <v>25</v>
@@ -19891,7 +19894,7 @@
         <v>238</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D214" s="4" t="s">
         <v>350</v>
@@ -19903,7 +19906,7 @@
         <v>678</v>
       </c>
       <c r="G214" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H214" s="4" t="s">
         <v>25</v>
@@ -19971,7 +19974,7 @@
         <v>240</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D215" s="4" t="s">
         <v>351</v>
@@ -19983,7 +19986,7 @@
         <v>678</v>
       </c>
       <c r="G215" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H215" s="4" t="s">
         <v>25</v>
@@ -20051,7 +20054,7 @@
         <v>242</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D216" s="4" t="s">
         <v>352</v>
@@ -20063,7 +20066,7 @@
         <v>678</v>
       </c>
       <c r="G216" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H216" s="4" t="s">
         <v>25</v>
@@ -20131,7 +20134,7 @@
         <v>244</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D217" s="4" t="s">
         <v>353</v>
@@ -20143,7 +20146,7 @@
         <v>678</v>
       </c>
       <c r="G217" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H217" s="4" t="s">
         <v>25</v>
@@ -27231,7 +27234,7 @@
         <v>210</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D308" s="4" t="s">
         <v>444</v>
@@ -27243,7 +27246,7 @@
         <v>678</v>
       </c>
       <c r="G308" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H308" s="4" t="s">
         <v>25</v>
@@ -27311,7 +27314,7 @@
         <v>212</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D309" s="4" t="s">
         <v>445</v>
@@ -27323,7 +27326,7 @@
         <v>678</v>
       </c>
       <c r="G309" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H309" s="4" t="s">
         <v>25</v>
@@ -27391,7 +27394,7 @@
         <v>214</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D310" s="4" t="s">
         <v>446</v>
@@ -27403,7 +27406,7 @@
         <v>678</v>
       </c>
       <c r="G310" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H310" s="4" t="s">
         <v>25</v>
@@ -27711,7 +27714,7 @@
         <v>222</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D314" s="4" t="s">
         <v>450</v>
@@ -27723,7 +27726,7 @@
         <v>678</v>
       </c>
       <c r="G314" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H314" s="4" t="s">
         <v>25</v>
@@ -27791,7 +27794,7 @@
         <v>224</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D315" s="4" t="s">
         <v>451</v>
@@ -27803,7 +27806,7 @@
         <v>678</v>
       </c>
       <c r="G315" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H315" s="4" t="s">
         <v>25</v>
@@ -27871,7 +27874,7 @@
         <v>226</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D316" s="4" t="s">
         <v>452</v>
@@ -27883,7 +27886,7 @@
         <v>678</v>
       </c>
       <c r="G316" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H316" s="4" t="s">
         <v>25</v>
@@ -28191,7 +28194,7 @@
         <v>234</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D320" s="4" t="s">
         <v>456</v>
@@ -28203,7 +28206,7 @@
         <v>678</v>
       </c>
       <c r="G320" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H320" s="4" t="s">
         <v>25</v>
@@ -28271,7 +28274,7 @@
         <v>236</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D321" s="4" t="s">
         <v>457</v>
@@ -28283,7 +28286,7 @@
         <v>678</v>
       </c>
       <c r="G321" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H321" s="4" t="s">
         <v>25</v>
@@ -28351,7 +28354,7 @@
         <v>238</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D322" s="4" t="s">
         <v>458</v>
@@ -28363,7 +28366,7 @@
         <v>678</v>
       </c>
       <c r="G322" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H322" s="4" t="s">
         <v>25</v>
@@ -28431,7 +28434,7 @@
         <v>240</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D323" s="4" t="s">
         <v>459</v>
@@ -28443,7 +28446,7 @@
         <v>678</v>
       </c>
       <c r="G323" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H323" s="4" t="s">
         <v>25</v>
@@ -28511,7 +28514,7 @@
         <v>242</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D324" s="4" t="s">
         <v>460</v>
@@ -28523,7 +28526,7 @@
         <v>678</v>
       </c>
       <c r="G324" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H324" s="4" t="s">
         <v>25</v>
@@ -28591,7 +28594,7 @@
         <v>244</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D325" s="4" t="s">
         <v>461</v>
@@ -28603,7 +28606,7 @@
         <v>678</v>
       </c>
       <c r="G325" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H325" s="4" t="s">
         <v>25</v>
@@ -35691,7 +35694,7 @@
         <v>210</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D416" s="4" t="s">
         <v>552</v>
@@ -35703,7 +35706,7 @@
         <v>678</v>
       </c>
       <c r="G416" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H416" s="4" t="s">
         <v>25</v>
@@ -35771,7 +35774,7 @@
         <v>212</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D417" s="4" t="s">
         <v>553</v>
@@ -35783,7 +35786,7 @@
         <v>678</v>
       </c>
       <c r="G417" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H417" s="4" t="s">
         <v>25</v>
@@ -35851,7 +35854,7 @@
         <v>214</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D418" s="4" t="s">
         <v>554</v>
@@ -35863,7 +35866,7 @@
         <v>678</v>
       </c>
       <c r="G418" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H418" s="4" t="s">
         <v>25</v>
@@ -36171,7 +36174,7 @@
         <v>222</v>
       </c>
       <c r="C422" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D422" s="4" t="s">
         <v>558</v>
@@ -36183,7 +36186,7 @@
         <v>678</v>
       </c>
       <c r="G422" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H422" s="4" t="s">
         <v>25</v>
@@ -36251,7 +36254,7 @@
         <v>224</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D423" s="4" t="s">
         <v>559</v>
@@ -36263,7 +36266,7 @@
         <v>678</v>
       </c>
       <c r="G423" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H423" s="4" t="s">
         <v>25</v>
@@ -36331,7 +36334,7 @@
         <v>226</v>
       </c>
       <c r="C424" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D424" s="4" t="s">
         <v>560</v>
@@ -36343,7 +36346,7 @@
         <v>678</v>
       </c>
       <c r="G424" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H424" s="4" t="s">
         <v>25</v>
@@ -36651,7 +36654,7 @@
         <v>234</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D428" s="4" t="s">
         <v>564</v>
@@ -36663,7 +36666,7 @@
         <v>678</v>
       </c>
       <c r="G428" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H428" s="4" t="s">
         <v>25</v>
@@ -36731,7 +36734,7 @@
         <v>236</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D429" s="4" t="s">
         <v>565</v>
@@ -36743,7 +36746,7 @@
         <v>678</v>
       </c>
       <c r="G429" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H429" s="4" t="s">
         <v>25</v>
@@ -36811,7 +36814,7 @@
         <v>238</v>
       </c>
       <c r="C430" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D430" s="4" t="s">
         <v>566</v>
@@ -36823,7 +36826,7 @@
         <v>678</v>
       </c>
       <c r="G430" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H430" s="4" t="s">
         <v>25</v>
@@ -36891,7 +36894,7 @@
         <v>240</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D431" s="4" t="s">
         <v>567</v>
@@ -36903,7 +36906,7 @@
         <v>678</v>
       </c>
       <c r="G431" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H431" s="4" t="s">
         <v>25</v>
@@ -36971,7 +36974,7 @@
         <v>242</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D432" s="4" t="s">
         <v>568</v>
@@ -36983,7 +36986,7 @@
         <v>678</v>
       </c>
       <c r="G432" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H432" s="4" t="s">
         <v>25</v>
@@ -37051,7 +37054,7 @@
         <v>244</v>
       </c>
       <c r="C433" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D433" s="4" t="s">
         <v>569</v>
@@ -37063,7 +37066,7 @@
         <v>678</v>
       </c>
       <c r="G433" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H433" s="4" t="s">
         <v>25</v>
@@ -44151,7 +44154,7 @@
         <v>210</v>
       </c>
       <c r="C524" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D524" s="4" t="s">
         <v>660</v>
@@ -44163,7 +44166,7 @@
         <v>678</v>
       </c>
       <c r="G524" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H524" s="4" t="s">
         <v>25</v>
@@ -44231,7 +44234,7 @@
         <v>212</v>
       </c>
       <c r="C525" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D525" s="4" t="s">
         <v>661</v>
@@ -44243,7 +44246,7 @@
         <v>678</v>
       </c>
       <c r="G525" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H525" s="4" t="s">
         <v>25</v>
@@ -44311,7 +44314,7 @@
         <v>214</v>
       </c>
       <c r="C526" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D526" s="4" t="s">
         <v>662</v>
@@ -44323,7 +44326,7 @@
         <v>678</v>
       </c>
       <c r="G526" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H526" s="4" t="s">
         <v>25</v>
@@ -44631,7 +44634,7 @@
         <v>222</v>
       </c>
       <c r="C530" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D530" s="4" t="s">
         <v>666</v>
@@ -44643,7 +44646,7 @@
         <v>678</v>
       </c>
       <c r="G530" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H530" s="4" t="s">
         <v>25</v>
@@ -44711,7 +44714,7 @@
         <v>224</v>
       </c>
       <c r="C531" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D531" s="4" t="s">
         <v>667</v>
@@ -44723,7 +44726,7 @@
         <v>678</v>
       </c>
       <c r="G531" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H531" s="4" t="s">
         <v>25</v>
@@ -44791,7 +44794,7 @@
         <v>226</v>
       </c>
       <c r="C532" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D532" s="4" t="s">
         <v>668</v>
@@ -44803,7 +44806,7 @@
         <v>678</v>
       </c>
       <c r="G532" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H532" s="4" t="s">
         <v>25</v>
@@ -45111,7 +45114,7 @@
         <v>234</v>
       </c>
       <c r="C536" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D536" s="4" t="s">
         <v>672</v>
@@ -45123,7 +45126,7 @@
         <v>678</v>
       </c>
       <c r="G536" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H536" s="4" t="s">
         <v>25</v>
@@ -45191,7 +45194,7 @@
         <v>236</v>
       </c>
       <c r="C537" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D537" s="4" t="s">
         <v>673</v>
@@ -45203,7 +45206,7 @@
         <v>678</v>
       </c>
       <c r="G537" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H537" s="4" t="s">
         <v>25</v>
@@ -45271,7 +45274,7 @@
         <v>238</v>
       </c>
       <c r="C538" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D538" s="4" t="s">
         <v>674</v>
@@ -45283,7 +45286,7 @@
         <v>678</v>
       </c>
       <c r="G538" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H538" s="4" t="s">
         <v>25</v>
@@ -45351,7 +45354,7 @@
         <v>240</v>
       </c>
       <c r="C539" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D539" s="4" t="s">
         <v>675</v>
@@ -45363,7 +45366,7 @@
         <v>678</v>
       </c>
       <c r="G539" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H539" s="4" t="s">
         <v>25</v>
@@ -45431,7 +45434,7 @@
         <v>242</v>
       </c>
       <c r="C540" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D540" s="4" t="s">
         <v>676</v>
@@ -45443,7 +45446,7 @@
         <v>678</v>
       </c>
       <c r="G540" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H540" s="4" t="s">
         <v>25</v>
@@ -45511,7 +45514,7 @@
         <v>244</v>
       </c>
       <c r="C541" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D541" s="4" t="s">
         <v>677</v>
@@ -45523,7 +45526,7 @@
         <v>678</v>
       </c>
       <c r="G541" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H541" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
working days december run v1
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
+++ b/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC787C-1556-4DAD-8BE7-C43BEBE8D05C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA5909A-8D50-4537-98ED-F1A8DC255E3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3195,7 +3195,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="91" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G200" sqref="G200:G541"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92:C541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10314,7 +10314,7 @@
         <v>210</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>211</v>
@@ -10394,7 +10394,7 @@
         <v>212</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>213</v>
@@ -10474,7 +10474,7 @@
         <v>214</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>215</v>
@@ -10794,7 +10794,7 @@
         <v>222</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>223</v>
@@ -10874,7 +10874,7 @@
         <v>224</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>225</v>
@@ -10954,7 +10954,7 @@
         <v>226</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>227</v>
@@ -11274,7 +11274,7 @@
         <v>234</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>235</v>
@@ -11354,7 +11354,7 @@
         <v>236</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>237</v>
@@ -11434,7 +11434,7 @@
         <v>238</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>239</v>
@@ -11514,7 +11514,7 @@
         <v>240</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>241</v>
@@ -11594,7 +11594,7 @@
         <v>242</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>243</v>
@@ -11674,7 +11674,7 @@
         <v>244</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>245</v>
@@ -18854,7 +18854,7 @@
         <v>212</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D201" s="4" t="s">
         <v>337</v>
@@ -18934,7 +18934,7 @@
         <v>214</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D202" s="4" t="s">
         <v>338</v>
@@ -19254,7 +19254,7 @@
         <v>222</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D206" s="4" t="s">
         <v>342</v>
@@ -19334,7 +19334,7 @@
         <v>224</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D207" s="4" t="s">
         <v>343</v>
@@ -19414,7 +19414,7 @@
         <v>226</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D208" s="4" t="s">
         <v>344</v>
@@ -19734,7 +19734,7 @@
         <v>234</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D212" s="4" t="s">
         <v>348</v>
@@ -19814,7 +19814,7 @@
         <v>236</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D213" s="4" t="s">
         <v>349</v>
@@ -19894,7 +19894,7 @@
         <v>238</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D214" s="4" t="s">
         <v>350</v>
@@ -19974,7 +19974,7 @@
         <v>240</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D215" s="4" t="s">
         <v>351</v>
@@ -20054,7 +20054,7 @@
         <v>242</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D216" s="4" t="s">
         <v>352</v>
@@ -20134,7 +20134,7 @@
         <v>244</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D217" s="4" t="s">
         <v>353</v>
@@ -27234,7 +27234,7 @@
         <v>210</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D308" s="4" t="s">
         <v>444</v>
@@ -27314,7 +27314,7 @@
         <v>212</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D309" s="4" t="s">
         <v>445</v>
@@ -27394,7 +27394,7 @@
         <v>214</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D310" s="4" t="s">
         <v>446</v>
@@ -27714,7 +27714,7 @@
         <v>222</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D314" s="4" t="s">
         <v>450</v>
@@ -27794,7 +27794,7 @@
         <v>224</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D315" s="4" t="s">
         <v>451</v>
@@ -27874,7 +27874,7 @@
         <v>226</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D316" s="4" t="s">
         <v>452</v>
@@ -28194,7 +28194,7 @@
         <v>234</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D320" s="4" t="s">
         <v>456</v>
@@ -28274,7 +28274,7 @@
         <v>236</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D321" s="4" t="s">
         <v>457</v>
@@ -28354,7 +28354,7 @@
         <v>238</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D322" s="4" t="s">
         <v>458</v>
@@ -28434,7 +28434,7 @@
         <v>240</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D323" s="4" t="s">
         <v>459</v>
@@ -28514,7 +28514,7 @@
         <v>242</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D324" s="4" t="s">
         <v>460</v>
@@ -28594,7 +28594,7 @@
         <v>244</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D325" s="4" t="s">
         <v>461</v>
@@ -35694,7 +35694,7 @@
         <v>210</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D416" s="4" t="s">
         <v>552</v>
@@ -35774,7 +35774,7 @@
         <v>212</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D417" s="4" t="s">
         <v>553</v>
@@ -35854,7 +35854,7 @@
         <v>214</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D418" s="4" t="s">
         <v>554</v>
@@ -36174,7 +36174,7 @@
         <v>222</v>
       </c>
       <c r="C422" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D422" s="4" t="s">
         <v>558</v>
@@ -36254,7 +36254,7 @@
         <v>224</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D423" s="4" t="s">
         <v>559</v>
@@ -36334,7 +36334,7 @@
         <v>226</v>
       </c>
       <c r="C424" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D424" s="4" t="s">
         <v>560</v>
@@ -36654,7 +36654,7 @@
         <v>234</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D428" s="4" t="s">
         <v>564</v>
@@ -36734,7 +36734,7 @@
         <v>236</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D429" s="4" t="s">
         <v>565</v>
@@ -36814,7 +36814,7 @@
         <v>238</v>
       </c>
       <c r="C430" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D430" s="4" t="s">
         <v>566</v>
@@ -36894,7 +36894,7 @@
         <v>240</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D431" s="4" t="s">
         <v>567</v>
@@ -36974,7 +36974,7 @@
         <v>242</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D432" s="4" t="s">
         <v>568</v>
@@ -37054,7 +37054,7 @@
         <v>244</v>
       </c>
       <c r="C433" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D433" s="4" t="s">
         <v>569</v>
@@ -44154,7 +44154,7 @@
         <v>210</v>
       </c>
       <c r="C524" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D524" s="4" t="s">
         <v>660</v>
@@ -44234,7 +44234,7 @@
         <v>212</v>
       </c>
       <c r="C525" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D525" s="4" t="s">
         <v>661</v>
@@ -44314,7 +44314,7 @@
         <v>214</v>
       </c>
       <c r="C526" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D526" s="4" t="s">
         <v>662</v>
@@ -44634,7 +44634,7 @@
         <v>222</v>
       </c>
       <c r="C530" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D530" s="4" t="s">
         <v>666</v>
@@ -44714,7 +44714,7 @@
         <v>224</v>
       </c>
       <c r="C531" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D531" s="4" t="s">
         <v>667</v>
@@ -44794,7 +44794,7 @@
         <v>226</v>
       </c>
       <c r="C532" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D532" s="4" t="s">
         <v>668</v>
@@ -45114,7 +45114,7 @@
         <v>234</v>
       </c>
       <c r="C536" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D536" s="4" t="s">
         <v>672</v>
@@ -45194,7 +45194,7 @@
         <v>236</v>
       </c>
       <c r="C537" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D537" s="4" t="s">
         <v>673</v>
@@ -45274,7 +45274,7 @@
         <v>238</v>
       </c>
       <c r="C538" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D538" s="4" t="s">
         <v>674</v>
@@ -45354,7 +45354,7 @@
         <v>240</v>
       </c>
       <c r="C539" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D539" s="4" t="s">
         <v>675</v>
@@ -45434,7 +45434,7 @@
         <v>242</v>
       </c>
       <c r="C540" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D540" s="4" t="s">
         <v>676</v>
@@ -45514,7 +45514,7 @@
         <v>244</v>
       </c>
       <c r="C541" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D541" s="4" t="s">
         <v>677</v>

</xml_diff>

<commit_message>
working days november  run v1
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
+++ b/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA5909A-8D50-4537-98ED-F1A8DC255E3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70265055-C01B-4550-BE0D-A6AB38293915}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2818,7 +2818,7 @@
     <t>january</t>
   </si>
   <si>
-    <t>december</t>
+    <t>november</t>
   </si>
 </sst>
 </file>
@@ -3195,7 +3195,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="91" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92:C541"/>
+      <selection pane="bottomLeft" activeCell="G92" sqref="G92:G541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10326,7 +10326,7 @@
         <v>678</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>25</v>
@@ -10406,7 +10406,7 @@
         <v>678</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>25</v>
@@ -10486,7 +10486,7 @@
         <v>678</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H94" s="4" t="s">
         <v>25</v>
@@ -10806,7 +10806,7 @@
         <v>678</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>25</v>
@@ -10886,7 +10886,7 @@
         <v>678</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>25</v>
@@ -10966,7 +10966,7 @@
         <v>678</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>25</v>
@@ -11286,7 +11286,7 @@
         <v>678</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>25</v>
@@ -11366,7 +11366,7 @@
         <v>678</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H105" s="4" t="s">
         <v>25</v>
@@ -11446,7 +11446,7 @@
         <v>678</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H106" s="4" t="s">
         <v>25</v>
@@ -11526,7 +11526,7 @@
         <v>678</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H107" s="4" t="s">
         <v>25</v>
@@ -11606,7 +11606,7 @@
         <v>678</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>25</v>
@@ -11686,7 +11686,7 @@
         <v>678</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H109" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
leave balance run - october
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
+++ b/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5945FF4C-D0B8-443E-899C-AE223B1567E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A758A497-A60E-430F-8B7B-099332ECFB33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="683">
   <si>
     <t>Test Case</t>
   </si>
@@ -2819,6 +2819,9 @@
   </si>
   <si>
     <t>november</t>
+  </si>
+  <si>
+    <t>october</t>
   </si>
 </sst>
 </file>
@@ -3195,7 +3198,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="91" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92:C541"/>
+      <selection pane="bottomLeft" activeCell="H541" sqref="H541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10326,7 +10329,7 @@
         <v>678</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>25</v>
@@ -10406,7 +10409,7 @@
         <v>678</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>25</v>
@@ -10486,7 +10489,7 @@
         <v>678</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H94" s="4" t="s">
         <v>25</v>
@@ -10806,7 +10809,7 @@
         <v>678</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>25</v>
@@ -10886,7 +10889,7 @@
         <v>678</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>25</v>
@@ -10966,7 +10969,7 @@
         <v>678</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>25</v>
@@ -11286,7 +11289,7 @@
         <v>678</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>25</v>
@@ -11366,7 +11369,7 @@
         <v>678</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H105" s="4" t="s">
         <v>25</v>
@@ -11446,7 +11449,7 @@
         <v>678</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H106" s="4" t="s">
         <v>25</v>
@@ -11526,7 +11529,7 @@
         <v>678</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H107" s="4" t="s">
         <v>25</v>
@@ -11606,7 +11609,7 @@
         <v>678</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>25</v>
@@ -11686,7 +11689,7 @@
         <v>678</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H109" s="4" t="s">
         <v>25</v>
@@ -27246,7 +27249,7 @@
         <v>678</v>
       </c>
       <c r="G308" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H308" s="4" t="s">
         <v>25</v>
@@ -27326,7 +27329,7 @@
         <v>678</v>
       </c>
       <c r="G309" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H309" s="4" t="s">
         <v>25</v>
@@ -27406,7 +27409,7 @@
         <v>678</v>
       </c>
       <c r="G310" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H310" s="4" t="s">
         <v>25</v>
@@ -27726,7 +27729,7 @@
         <v>678</v>
       </c>
       <c r="G314" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H314" s="4" t="s">
         <v>25</v>
@@ -27806,7 +27809,7 @@
         <v>678</v>
       </c>
       <c r="G315" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H315" s="4" t="s">
         <v>25</v>
@@ -27886,7 +27889,7 @@
         <v>678</v>
       </c>
       <c r="G316" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H316" s="4" t="s">
         <v>25</v>
@@ -28206,7 +28209,7 @@
         <v>678</v>
       </c>
       <c r="G320" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H320" s="4" t="s">
         <v>25</v>
@@ -28286,7 +28289,7 @@
         <v>678</v>
       </c>
       <c r="G321" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H321" s="4" t="s">
         <v>25</v>
@@ -28366,7 +28369,7 @@
         <v>678</v>
       </c>
       <c r="G322" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H322" s="4" t="s">
         <v>25</v>
@@ -28446,7 +28449,7 @@
         <v>678</v>
       </c>
       <c r="G323" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H323" s="4" t="s">
         <v>25</v>
@@ -28526,7 +28529,7 @@
         <v>678</v>
       </c>
       <c r="G324" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H324" s="4" t="s">
         <v>25</v>
@@ -28606,7 +28609,7 @@
         <v>678</v>
       </c>
       <c r="G325" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H325" s="4" t="s">
         <v>25</v>
@@ -35706,7 +35709,7 @@
         <v>678</v>
       </c>
       <c r="G416" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H416" s="4" t="s">
         <v>25</v>
@@ -35786,7 +35789,7 @@
         <v>678</v>
       </c>
       <c r="G417" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H417" s="4" t="s">
         <v>25</v>
@@ -35866,7 +35869,7 @@
         <v>678</v>
       </c>
       <c r="G418" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H418" s="4" t="s">
         <v>25</v>
@@ -36186,7 +36189,7 @@
         <v>678</v>
       </c>
       <c r="G422" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H422" s="4" t="s">
         <v>25</v>
@@ -36266,7 +36269,7 @@
         <v>678</v>
       </c>
       <c r="G423" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H423" s="4" t="s">
         <v>25</v>
@@ -36346,7 +36349,7 @@
         <v>678</v>
       </c>
       <c r="G424" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H424" s="4" t="s">
         <v>25</v>
@@ -36666,7 +36669,7 @@
         <v>678</v>
       </c>
       <c r="G428" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H428" s="4" t="s">
         <v>25</v>
@@ -36746,7 +36749,7 @@
         <v>678</v>
       </c>
       <c r="G429" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H429" s="4" t="s">
         <v>25</v>
@@ -36826,7 +36829,7 @@
         <v>678</v>
       </c>
       <c r="G430" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H430" s="4" t="s">
         <v>25</v>
@@ -36906,7 +36909,7 @@
         <v>678</v>
       </c>
       <c r="G431" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H431" s="4" t="s">
         <v>25</v>
@@ -36986,7 +36989,7 @@
         <v>678</v>
       </c>
       <c r="G432" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H432" s="4" t="s">
         <v>25</v>
@@ -37066,7 +37069,7 @@
         <v>678</v>
       </c>
       <c r="G433" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H433" s="4" t="s">
         <v>25</v>
@@ -44166,7 +44169,7 @@
         <v>678</v>
       </c>
       <c r="G524" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H524" s="4" t="s">
         <v>25</v>
@@ -44246,7 +44249,7 @@
         <v>678</v>
       </c>
       <c r="G525" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H525" s="4" t="s">
         <v>25</v>
@@ -44326,7 +44329,7 @@
         <v>678</v>
       </c>
       <c r="G526" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H526" s="4" t="s">
         <v>25</v>
@@ -44646,7 +44649,7 @@
         <v>678</v>
       </c>
       <c r="G530" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H530" s="4" t="s">
         <v>25</v>
@@ -44726,7 +44729,7 @@
         <v>678</v>
       </c>
       <c r="G531" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H531" s="4" t="s">
         <v>25</v>
@@ -44806,7 +44809,7 @@
         <v>678</v>
       </c>
       <c r="G532" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H532" s="4" t="s">
         <v>25</v>
@@ -45126,7 +45129,7 @@
         <v>678</v>
       </c>
       <c r="G536" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H536" s="4" t="s">
         <v>25</v>
@@ -45206,7 +45209,7 @@
         <v>678</v>
       </c>
       <c r="G537" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H537" s="4" t="s">
         <v>25</v>
@@ -45286,7 +45289,7 @@
         <v>678</v>
       </c>
       <c r="G538" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H538" s="4" t="s">
         <v>25</v>
@@ -45366,7 +45369,7 @@
         <v>678</v>
       </c>
       <c r="G539" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H539" s="4" t="s">
         <v>25</v>
@@ -45446,7 +45449,7 @@
         <v>678</v>
       </c>
       <c r="G540" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H540" s="4" t="s">
         <v>25</v>
@@ -45526,7 +45529,7 @@
         <v>678</v>
       </c>
       <c r="G541" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H541" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
working days - november failed case rerun
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
+++ b/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A758A497-A60E-430F-8B7B-099332ECFB33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B2ADF1-D93A-4E7C-A48F-B01B840A49A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="682">
   <si>
     <t>Test Case</t>
   </si>
@@ -2819,9 +2819,6 @@
   </si>
   <si>
     <t>november</t>
-  </si>
-  <si>
-    <t>october</t>
   </si>
 </sst>
 </file>
@@ -3196,9 +3193,9 @@
   <dimension ref="A1:Z541"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="91" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="91" topLeftCell="A433" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H541" sqref="H541"/>
+      <selection pane="bottomLeft" activeCell="J433" sqref="J433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10317,7 +10314,7 @@
         <v>210</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>211</v>
@@ -10329,7 +10326,7 @@
         <v>678</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>25</v>
@@ -10397,7 +10394,7 @@
         <v>212</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>213</v>
@@ -10409,7 +10406,7 @@
         <v>678</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>25</v>
@@ -10477,7 +10474,7 @@
         <v>214</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>215</v>
@@ -10489,7 +10486,7 @@
         <v>678</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H94" s="4" t="s">
         <v>25</v>
@@ -10797,7 +10794,7 @@
         <v>222</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>223</v>
@@ -10809,7 +10806,7 @@
         <v>678</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>25</v>
@@ -10877,7 +10874,7 @@
         <v>224</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>225</v>
@@ -10889,7 +10886,7 @@
         <v>678</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>25</v>
@@ -10957,7 +10954,7 @@
         <v>226</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>227</v>
@@ -10969,7 +10966,7 @@
         <v>678</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>25</v>
@@ -11277,7 +11274,7 @@
         <v>234</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>235</v>
@@ -11289,7 +11286,7 @@
         <v>678</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>25</v>
@@ -11357,7 +11354,7 @@
         <v>236</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>237</v>
@@ -11369,7 +11366,7 @@
         <v>678</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H105" s="4" t="s">
         <v>25</v>
@@ -11437,7 +11434,7 @@
         <v>238</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>239</v>
@@ -11449,7 +11446,7 @@
         <v>678</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H106" s="4" t="s">
         <v>25</v>
@@ -11517,7 +11514,7 @@
         <v>240</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>241</v>
@@ -11529,7 +11526,7 @@
         <v>678</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H107" s="4" t="s">
         <v>25</v>
@@ -11597,7 +11594,7 @@
         <v>242</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>243</v>
@@ -11609,7 +11606,7 @@
         <v>678</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>25</v>
@@ -11677,7 +11674,7 @@
         <v>244</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>245</v>
@@ -11689,7 +11686,7 @@
         <v>678</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H109" s="4" t="s">
         <v>25</v>
@@ -27237,7 +27234,7 @@
         <v>210</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D308" s="4" t="s">
         <v>444</v>
@@ -27249,7 +27246,7 @@
         <v>678</v>
       </c>
       <c r="G308" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H308" s="4" t="s">
         <v>25</v>
@@ -27317,7 +27314,7 @@
         <v>212</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D309" s="4" t="s">
         <v>445</v>
@@ -27329,7 +27326,7 @@
         <v>678</v>
       </c>
       <c r="G309" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H309" s="4" t="s">
         <v>25</v>
@@ -27397,7 +27394,7 @@
         <v>214</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D310" s="4" t="s">
         <v>446</v>
@@ -27409,7 +27406,7 @@
         <v>678</v>
       </c>
       <c r="G310" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H310" s="4" t="s">
         <v>25</v>
@@ -27717,7 +27714,7 @@
         <v>222</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D314" s="4" t="s">
         <v>450</v>
@@ -27729,7 +27726,7 @@
         <v>678</v>
       </c>
       <c r="G314" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H314" s="4" t="s">
         <v>25</v>
@@ -27797,7 +27794,7 @@
         <v>224</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D315" s="4" t="s">
         <v>451</v>
@@ -27809,7 +27806,7 @@
         <v>678</v>
       </c>
       <c r="G315" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H315" s="4" t="s">
         <v>25</v>
@@ -27877,7 +27874,7 @@
         <v>226</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D316" s="4" t="s">
         <v>452</v>
@@ -27889,7 +27886,7 @@
         <v>678</v>
       </c>
       <c r="G316" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H316" s="4" t="s">
         <v>25</v>
@@ -28197,7 +28194,7 @@
         <v>234</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D320" s="4" t="s">
         <v>456</v>
@@ -28209,7 +28206,7 @@
         <v>678</v>
       </c>
       <c r="G320" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H320" s="4" t="s">
         <v>25</v>
@@ -28277,7 +28274,7 @@
         <v>236</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D321" s="4" t="s">
         <v>457</v>
@@ -28289,7 +28286,7 @@
         <v>678</v>
       </c>
       <c r="G321" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H321" s="4" t="s">
         <v>25</v>
@@ -28357,7 +28354,7 @@
         <v>238</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D322" s="4" t="s">
         <v>458</v>
@@ -28369,7 +28366,7 @@
         <v>678</v>
       </c>
       <c r="G322" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H322" s="4" t="s">
         <v>25</v>
@@ -28437,7 +28434,7 @@
         <v>240</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D323" s="4" t="s">
         <v>459</v>
@@ -28449,7 +28446,7 @@
         <v>678</v>
       </c>
       <c r="G323" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H323" s="4" t="s">
         <v>25</v>
@@ -28517,7 +28514,7 @@
         <v>242</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D324" s="4" t="s">
         <v>460</v>
@@ -28529,7 +28526,7 @@
         <v>678</v>
       </c>
       <c r="G324" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H324" s="4" t="s">
         <v>25</v>
@@ -28597,7 +28594,7 @@
         <v>244</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D325" s="4" t="s">
         <v>461</v>
@@ -28609,7 +28606,7 @@
         <v>678</v>
       </c>
       <c r="G325" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H325" s="4" t="s">
         <v>25</v>
@@ -35709,7 +35706,7 @@
         <v>678</v>
       </c>
       <c r="G416" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H416" s="4" t="s">
         <v>25</v>
@@ -35789,7 +35786,7 @@
         <v>678</v>
       </c>
       <c r="G417" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H417" s="4" t="s">
         <v>25</v>
@@ -35869,7 +35866,7 @@
         <v>678</v>
       </c>
       <c r="G418" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H418" s="4" t="s">
         <v>25</v>
@@ -36189,7 +36186,7 @@
         <v>678</v>
       </c>
       <c r="G422" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H422" s="4" t="s">
         <v>25</v>
@@ -36269,7 +36266,7 @@
         <v>678</v>
       </c>
       <c r="G423" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H423" s="4" t="s">
         <v>25</v>
@@ -36349,7 +36346,7 @@
         <v>678</v>
       </c>
       <c r="G424" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H424" s="4" t="s">
         <v>25</v>
@@ -36669,7 +36666,7 @@
         <v>678</v>
       </c>
       <c r="G428" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H428" s="4" t="s">
         <v>25</v>
@@ -36749,7 +36746,7 @@
         <v>678</v>
       </c>
       <c r="G429" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H429" s="4" t="s">
         <v>25</v>
@@ -36829,7 +36826,7 @@
         <v>678</v>
       </c>
       <c r="G430" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H430" s="4" t="s">
         <v>25</v>
@@ -36909,7 +36906,7 @@
         <v>678</v>
       </c>
       <c r="G431" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H431" s="4" t="s">
         <v>25</v>
@@ -36989,7 +36986,7 @@
         <v>678</v>
       </c>
       <c r="G432" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H432" s="4" t="s">
         <v>25</v>
@@ -37069,7 +37066,7 @@
         <v>678</v>
       </c>
       <c r="G433" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H433" s="4" t="s">
         <v>25</v>
@@ -44157,7 +44154,7 @@
         <v>210</v>
       </c>
       <c r="C524" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D524" s="4" t="s">
         <v>660</v>
@@ -44169,7 +44166,7 @@
         <v>678</v>
       </c>
       <c r="G524" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H524" s="4" t="s">
         <v>25</v>
@@ -44237,7 +44234,7 @@
         <v>212</v>
       </c>
       <c r="C525" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D525" s="4" t="s">
         <v>661</v>
@@ -44249,7 +44246,7 @@
         <v>678</v>
       </c>
       <c r="G525" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H525" s="4" t="s">
         <v>25</v>
@@ -44317,7 +44314,7 @@
         <v>214</v>
       </c>
       <c r="C526" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D526" s="4" t="s">
         <v>662</v>
@@ -44329,7 +44326,7 @@
         <v>678</v>
       </c>
       <c r="G526" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H526" s="4" t="s">
         <v>25</v>
@@ -44637,7 +44634,7 @@
         <v>222</v>
       </c>
       <c r="C530" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D530" s="4" t="s">
         <v>666</v>
@@ -44649,7 +44646,7 @@
         <v>678</v>
       </c>
       <c r="G530" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H530" s="4" t="s">
         <v>25</v>
@@ -44717,7 +44714,7 @@
         <v>224</v>
       </c>
       <c r="C531" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D531" s="4" t="s">
         <v>667</v>
@@ -44729,7 +44726,7 @@
         <v>678</v>
       </c>
       <c r="G531" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H531" s="4" t="s">
         <v>25</v>
@@ -44797,7 +44794,7 @@
         <v>226</v>
       </c>
       <c r="C532" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D532" s="4" t="s">
         <v>668</v>
@@ -44809,7 +44806,7 @@
         <v>678</v>
       </c>
       <c r="G532" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H532" s="4" t="s">
         <v>25</v>
@@ -45117,7 +45114,7 @@
         <v>234</v>
       </c>
       <c r="C536" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D536" s="4" t="s">
         <v>672</v>
@@ -45129,7 +45126,7 @@
         <v>678</v>
       </c>
       <c r="G536" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H536" s="4" t="s">
         <v>25</v>
@@ -45197,7 +45194,7 @@
         <v>236</v>
       </c>
       <c r="C537" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D537" s="4" t="s">
         <v>673</v>
@@ -45209,7 +45206,7 @@
         <v>678</v>
       </c>
       <c r="G537" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H537" s="4" t="s">
         <v>25</v>
@@ -45277,7 +45274,7 @@
         <v>238</v>
       </c>
       <c r="C538" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D538" s="4" t="s">
         <v>674</v>
@@ -45289,7 +45286,7 @@
         <v>678</v>
       </c>
       <c r="G538" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H538" s="4" t="s">
         <v>25</v>
@@ -45357,7 +45354,7 @@
         <v>240</v>
       </c>
       <c r="C539" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D539" s="4" t="s">
         <v>675</v>
@@ -45369,7 +45366,7 @@
         <v>678</v>
       </c>
       <c r="G539" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H539" s="4" t="s">
         <v>25</v>
@@ -45437,7 +45434,7 @@
         <v>242</v>
       </c>
       <c r="C540" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D540" s="4" t="s">
         <v>676</v>
@@ -45449,7 +45446,7 @@
         <v>678</v>
       </c>
       <c r="G540" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H540" s="4" t="s">
         <v>25</v>
@@ -45517,7 +45514,7 @@
         <v>244</v>
       </c>
       <c r="C541" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D541" s="4" t="s">
         <v>677</v>
@@ -45529,7 +45526,7 @@
         <v>678</v>
       </c>
       <c r="G541" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H541" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
working days - october run
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
+++ b/leave/src/main/resources/TestData/Accural/WorkingDays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B2ADF1-D93A-4E7C-A48F-B01B840A49A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BAC44D-F68F-4931-9231-90257338A2CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="683">
   <si>
     <t>Test Case</t>
   </si>
@@ -2819,6 +2819,9 @@
   </si>
   <si>
     <t>november</t>
+  </si>
+  <si>
+    <t>october</t>
   </si>
 </sst>
 </file>
@@ -3193,9 +3196,9 @@
   <dimension ref="A1:Z541"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="91" topLeftCell="A433" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="91" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="J433" sqref="J433"/>
+      <selection pane="bottomLeft" activeCell="G92" sqref="G92:G541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10314,7 +10317,7 @@
         <v>210</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>211</v>
@@ -10326,7 +10329,7 @@
         <v>678</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>25</v>
@@ -10394,7 +10397,7 @@
         <v>212</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>213</v>
@@ -10406,7 +10409,7 @@
         <v>678</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>25</v>
@@ -10474,7 +10477,7 @@
         <v>214</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>215</v>
@@ -10486,7 +10489,7 @@
         <v>678</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H94" s="4" t="s">
         <v>25</v>
@@ -10794,7 +10797,7 @@
         <v>222</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>223</v>
@@ -10806,7 +10809,7 @@
         <v>678</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>25</v>
@@ -10874,7 +10877,7 @@
         <v>224</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>225</v>
@@ -10886,7 +10889,7 @@
         <v>678</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>25</v>
@@ -10954,7 +10957,7 @@
         <v>226</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>227</v>
@@ -10966,7 +10969,7 @@
         <v>678</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>25</v>
@@ -11274,7 +11277,7 @@
         <v>234</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>235</v>
@@ -11286,7 +11289,7 @@
         <v>678</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>25</v>
@@ -11354,7 +11357,7 @@
         <v>236</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>237</v>
@@ -11366,7 +11369,7 @@
         <v>678</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H105" s="4" t="s">
         <v>25</v>
@@ -11434,7 +11437,7 @@
         <v>238</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>239</v>
@@ -11446,7 +11449,7 @@
         <v>678</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H106" s="4" t="s">
         <v>25</v>
@@ -11514,7 +11517,7 @@
         <v>240</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>241</v>
@@ -11526,7 +11529,7 @@
         <v>678</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H107" s="4" t="s">
         <v>25</v>
@@ -11594,7 +11597,7 @@
         <v>242</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>243</v>
@@ -11606,7 +11609,7 @@
         <v>678</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>25</v>
@@ -11674,7 +11677,7 @@
         <v>244</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>245</v>
@@ -11686,7 +11689,7 @@
         <v>678</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H109" s="4" t="s">
         <v>25</v>
@@ -27234,7 +27237,7 @@
         <v>210</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D308" s="4" t="s">
         <v>444</v>
@@ -27246,7 +27249,7 @@
         <v>678</v>
       </c>
       <c r="G308" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H308" s="4" t="s">
         <v>25</v>
@@ -27314,7 +27317,7 @@
         <v>212</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D309" s="4" t="s">
         <v>445</v>
@@ -27326,7 +27329,7 @@
         <v>678</v>
       </c>
       <c r="G309" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H309" s="4" t="s">
         <v>25</v>
@@ -27394,7 +27397,7 @@
         <v>214</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D310" s="4" t="s">
         <v>446</v>
@@ -27406,7 +27409,7 @@
         <v>678</v>
       </c>
       <c r="G310" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H310" s="4" t="s">
         <v>25</v>
@@ -27714,7 +27717,7 @@
         <v>222</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D314" s="4" t="s">
         <v>450</v>
@@ -27726,7 +27729,7 @@
         <v>678</v>
       </c>
       <c r="G314" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H314" s="4" t="s">
         <v>25</v>
@@ -27794,7 +27797,7 @@
         <v>224</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D315" s="4" t="s">
         <v>451</v>
@@ -27806,7 +27809,7 @@
         <v>678</v>
       </c>
       <c r="G315" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H315" s="4" t="s">
         <v>25</v>
@@ -27874,7 +27877,7 @@
         <v>226</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D316" s="4" t="s">
         <v>452</v>
@@ -27886,7 +27889,7 @@
         <v>678</v>
       </c>
       <c r="G316" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H316" s="4" t="s">
         <v>25</v>
@@ -28194,7 +28197,7 @@
         <v>234</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D320" s="4" t="s">
         <v>456</v>
@@ -28206,7 +28209,7 @@
         <v>678</v>
       </c>
       <c r="G320" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H320" s="4" t="s">
         <v>25</v>
@@ -28274,7 +28277,7 @@
         <v>236</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D321" s="4" t="s">
         <v>457</v>
@@ -28286,7 +28289,7 @@
         <v>678</v>
       </c>
       <c r="G321" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H321" s="4" t="s">
         <v>25</v>
@@ -28354,7 +28357,7 @@
         <v>238</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D322" s="4" t="s">
         <v>458</v>
@@ -28366,7 +28369,7 @@
         <v>678</v>
       </c>
       <c r="G322" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H322" s="4" t="s">
         <v>25</v>
@@ -28434,7 +28437,7 @@
         <v>240</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D323" s="4" t="s">
         <v>459</v>
@@ -28446,7 +28449,7 @@
         <v>678</v>
       </c>
       <c r="G323" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H323" s="4" t="s">
         <v>25</v>
@@ -28514,7 +28517,7 @@
         <v>242</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D324" s="4" t="s">
         <v>460</v>
@@ -28526,7 +28529,7 @@
         <v>678</v>
       </c>
       <c r="G324" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H324" s="4" t="s">
         <v>25</v>
@@ -28594,7 +28597,7 @@
         <v>244</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D325" s="4" t="s">
         <v>461</v>
@@ -28606,7 +28609,7 @@
         <v>678</v>
       </c>
       <c r="G325" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H325" s="4" t="s">
         <v>25</v>
@@ -35706,7 +35709,7 @@
         <v>678</v>
       </c>
       <c r="G416" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H416" s="4" t="s">
         <v>25</v>
@@ -35786,7 +35789,7 @@
         <v>678</v>
       </c>
       <c r="G417" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H417" s="4" t="s">
         <v>25</v>
@@ -35866,7 +35869,7 @@
         <v>678</v>
       </c>
       <c r="G418" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H418" s="4" t="s">
         <v>25</v>
@@ -36186,7 +36189,7 @@
         <v>678</v>
       </c>
       <c r="G422" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H422" s="4" t="s">
         <v>25</v>
@@ -36266,7 +36269,7 @@
         <v>678</v>
       </c>
       <c r="G423" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H423" s="4" t="s">
         <v>25</v>
@@ -36346,7 +36349,7 @@
         <v>678</v>
       </c>
       <c r="G424" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H424" s="4" t="s">
         <v>25</v>
@@ -36666,7 +36669,7 @@
         <v>678</v>
       </c>
       <c r="G428" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H428" s="4" t="s">
         <v>25</v>
@@ -36746,7 +36749,7 @@
         <v>678</v>
       </c>
       <c r="G429" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H429" s="4" t="s">
         <v>25</v>
@@ -36826,7 +36829,7 @@
         <v>678</v>
       </c>
       <c r="G430" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H430" s="4" t="s">
         <v>25</v>
@@ -36906,7 +36909,7 @@
         <v>678</v>
       </c>
       <c r="G431" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H431" s="4" t="s">
         <v>25</v>
@@ -36986,7 +36989,7 @@
         <v>678</v>
       </c>
       <c r="G432" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H432" s="4" t="s">
         <v>25</v>
@@ -37066,7 +37069,7 @@
         <v>678</v>
       </c>
       <c r="G433" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H433" s="4" t="s">
         <v>25</v>
@@ -44154,7 +44157,7 @@
         <v>210</v>
       </c>
       <c r="C524" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D524" s="4" t="s">
         <v>660</v>
@@ -44166,7 +44169,7 @@
         <v>678</v>
       </c>
       <c r="G524" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H524" s="4" t="s">
         <v>25</v>
@@ -44234,7 +44237,7 @@
         <v>212</v>
       </c>
       <c r="C525" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D525" s="4" t="s">
         <v>661</v>
@@ -44246,7 +44249,7 @@
         <v>678</v>
       </c>
       <c r="G525" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H525" s="4" t="s">
         <v>25</v>
@@ -44314,7 +44317,7 @@
         <v>214</v>
       </c>
       <c r="C526" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D526" s="4" t="s">
         <v>662</v>
@@ -44326,7 +44329,7 @@
         <v>678</v>
       </c>
       <c r="G526" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H526" s="4" t="s">
         <v>25</v>
@@ -44634,7 +44637,7 @@
         <v>222</v>
       </c>
       <c r="C530" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D530" s="4" t="s">
         <v>666</v>
@@ -44646,7 +44649,7 @@
         <v>678</v>
       </c>
       <c r="G530" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H530" s="4" t="s">
         <v>25</v>
@@ -44714,7 +44717,7 @@
         <v>224</v>
       </c>
       <c r="C531" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D531" s="4" t="s">
         <v>667</v>
@@ -44726,7 +44729,7 @@
         <v>678</v>
       </c>
       <c r="G531" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H531" s="4" t="s">
         <v>25</v>
@@ -44794,7 +44797,7 @@
         <v>226</v>
       </c>
       <c r="C532" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D532" s="4" t="s">
         <v>668</v>
@@ -44806,7 +44809,7 @@
         <v>678</v>
       </c>
       <c r="G532" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H532" s="4" t="s">
         <v>25</v>
@@ -45114,7 +45117,7 @@
         <v>234</v>
       </c>
       <c r="C536" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D536" s="4" t="s">
         <v>672</v>
@@ -45126,7 +45129,7 @@
         <v>678</v>
       </c>
       <c r="G536" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H536" s="4" t="s">
         <v>25</v>
@@ -45194,7 +45197,7 @@
         <v>236</v>
       </c>
       <c r="C537" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D537" s="4" t="s">
         <v>673</v>
@@ -45206,7 +45209,7 @@
         <v>678</v>
       </c>
       <c r="G537" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H537" s="4" t="s">
         <v>25</v>
@@ -45274,7 +45277,7 @@
         <v>238</v>
       </c>
       <c r="C538" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D538" s="4" t="s">
         <v>674</v>
@@ -45286,7 +45289,7 @@
         <v>678</v>
       </c>
       <c r="G538" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H538" s="4" t="s">
         <v>25</v>
@@ -45354,7 +45357,7 @@
         <v>240</v>
       </c>
       <c r="C539" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D539" s="4" t="s">
         <v>675</v>
@@ -45366,7 +45369,7 @@
         <v>678</v>
       </c>
       <c r="G539" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H539" s="4" t="s">
         <v>25</v>
@@ -45434,7 +45437,7 @@
         <v>242</v>
       </c>
       <c r="C540" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D540" s="4" t="s">
         <v>676</v>
@@ -45446,7 +45449,7 @@
         <v>678</v>
       </c>
       <c r="G540" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H540" s="4" t="s">
         <v>25</v>
@@ -45514,7 +45517,7 @@
         <v>244</v>
       </c>
       <c r="C541" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D541" s="4" t="s">
         <v>677</v>
@@ -45526,7 +45529,7 @@
         <v>678</v>
       </c>
       <c r="G541" s="4" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H541" s="4" t="s">
         <v>25</v>

</xml_diff>